<commit_message>
update story board wire frame and data
</commit_message>
<xml_diff>
--- a/data/costdetails_convenient.xlsx
+++ b/data/costdetails_convenient.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunaynaagarwal/Documents/GitHub/capstone project/urbanforest_CBA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunaynaagarwal/Documents/GitHub/capstone project/urbanforest_CBA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE788DC-3058-5C48-AC90-81F3428716C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87270796-3D8A-3246-9896-91F1D9592CC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="940" yWindow="620" windowWidth="24640" windowHeight="13600" xr2:uid="{F848FDC7-4122-A740-B3C1-B5DA81FA0842}"/>
   </bookViews>
@@ -35,9 +35,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>installtion cost</t>
-  </si>
-  <si>
     <t>irrigation cost</t>
   </si>
   <si>
@@ -56,13 +53,16 @@
     <t>liability_legal cost</t>
   </si>
   <si>
-    <t>cost_description</t>
-  </si>
-  <si>
-    <t>first_year_$</t>
-  </si>
-  <si>
-    <t>yearly_cost_$</t>
+    <t>Cost Breakdown</t>
+  </si>
+  <si>
+    <t>Cost_First Year</t>
+  </si>
+  <si>
+    <t>Cost_Yearly</t>
+  </si>
+  <si>
+    <t>Convenient Installtion cost</t>
   </si>
 </sst>
 </file>
@@ -417,7 +417,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -429,21 +429,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B2">
-        <v>-510</v>
+        <v>510</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -459,7 +459,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>12</v>
@@ -467,7 +467,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>2.5</v>
@@ -475,7 +475,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -483,7 +483,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>0.01</v>
@@ -491,7 +491,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>0.01</v>

</xml_diff>